<commit_message>
FIRST SET OF RESULTS WITH TEST_DATA OF 8 PATIENTS
</commit_message>
<xml_diff>
--- a/src/Experiments_FINAL.xlsx
+++ b/src/Experiments_FINAL.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="11">
   <si>
     <t>103</t>
   </si>
@@ -26,6 +26,21 @@
   </si>
   <si>
     <t>151</t>
+  </si>
+  <si>
+    <t>165</t>
+  </si>
+  <si>
+    <t>176</t>
+  </si>
+  <si>
+    <t>219</t>
+  </si>
+  <si>
+    <t>230</t>
+  </si>
+  <si>
+    <t>255</t>
   </si>
   <si>
     <t>enhancing</t>
@@ -383,7 +398,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -391,7 +406,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:9">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -401,10 +416,25 @@
       <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:4">
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
       <c r="A2" s="1" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="B2" t="n">
         <v>0.7449211908931699</v>
@@ -415,10 +445,25 @@
       <c r="D2" t="n">
         <v>0.7532971138892816</v>
       </c>
-    </row>
-    <row r="3" spans="1:4">
+      <c r="E2" t="n">
+        <v>0.6767942583732057</v>
+      </c>
+      <c r="F2" t="n">
+        <v>0.8659619528869733</v>
+      </c>
+      <c r="G2" t="n">
+        <v>0.1046486298087396</v>
+      </c>
+      <c r="H2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2" t="n">
+        <v>0.0636084985984124</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
       <c r="A3" s="1" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="B3" t="n">
         <v>0.8174361581430529</v>
@@ -429,10 +474,25 @@
       <c r="D3" t="n">
         <v>0.6753345114869982</v>
       </c>
-    </row>
-    <row r="4" spans="1:4">
+      <c r="E3" t="n">
+        <v>0.2240525625420985</v>
+      </c>
+      <c r="F3" t="n">
+        <v>0.8110732931652131</v>
+      </c>
+      <c r="G3" t="n">
+        <v>0.07988905465319072</v>
+      </c>
+      <c r="H3" t="n">
+        <v>0.3538156692436423</v>
+      </c>
+      <c r="I3" t="n">
+        <v>0.6653323217601373</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
       <c r="A4" s="1" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="B4" t="n">
         <v>0.2773033707865168</v>
@@ -442,6 +502,21 @@
       </c>
       <c r="D4" t="n">
         <v>0.1785561725758223</v>
+      </c>
+      <c r="E4" t="n">
+        <v>0.1878588005374374</v>
+      </c>
+      <c r="F4" t="n">
+        <v>0.8384741106513197</v>
+      </c>
+      <c r="G4" t="n">
+        <v>0.4420361032894593</v>
+      </c>
+      <c r="H4" t="n">
+        <v>0.4851463183440783</v>
+      </c>
+      <c r="I4" t="n">
+        <v>0.7169509614167103</v>
       </c>
     </row>
   </sheetData>
@@ -455,7 +530,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -463,7 +538,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:9">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -473,47 +548,107 @@
       <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:4">
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
       <c r="A2" s="1" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="B2" t="n">
-        <v>0.3896574534786735</v>
+        <v>0.5511376545814535</v>
       </c>
       <c r="C2" t="n">
-        <v>0.5824197466027703</v>
+        <v>0.7403166869671133</v>
       </c>
       <c r="D2" t="n">
-        <v>0.6771276504125257</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
+        <v>0.8548771955004575</v>
+      </c>
+      <c r="E2" t="n">
+        <v>0.7045908183632734</v>
+      </c>
+      <c r="F2" t="n">
+        <v>0.8538366619441524</v>
+      </c>
+      <c r="G2" t="n">
+        <v>0.06291125020060985</v>
+      </c>
+      <c r="H2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2" t="n">
+        <v>0.0446162832744569</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
       <c r="A3" s="1" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="B3" t="n">
-        <v>0.3322213466201059</v>
+        <v>0.3350805603868428</v>
       </c>
       <c r="C3" t="n">
-        <v>0.1794007137057946</v>
+        <v>0.2651338453581083</v>
       </c>
       <c r="D3" t="n">
-        <v>0.2564226128068039</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
+        <v>0.2666733198369023</v>
+      </c>
+      <c r="E3" t="n">
+        <v>0.207284754882557</v>
+      </c>
+      <c r="F3" t="n">
+        <v>0.7782596172959202</v>
+      </c>
+      <c r="G3" t="n">
+        <v>0.03953029831325686</v>
+      </c>
+      <c r="H3" t="n">
+        <v>0.2034891273284664</v>
+      </c>
+      <c r="I3" t="n">
+        <v>0.2670860790301472</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
       <c r="A4" s="1" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="B4" t="n">
-        <v>0.05872369314324508</v>
+        <v>0.09595175327723809</v>
       </c>
       <c r="C4" t="n">
-        <v>0.1028445339857054</v>
+        <v>0.4426125554850983</v>
       </c>
       <c r="D4" t="n">
-        <v>0.0225362407114143</v>
+        <v>0.06573705179282868</v>
+      </c>
+      <c r="E4" t="n">
+        <v>0.1227107772807832</v>
+      </c>
+      <c r="F4" t="n">
+        <v>0.7151974233567935</v>
+      </c>
+      <c r="G4" t="n">
+        <v>0.2360949233364733</v>
+      </c>
+      <c r="H4" t="n">
+        <v>0.477882797731569</v>
+      </c>
+      <c r="I4" t="n">
+        <v>0.544350779374509</v>
       </c>
     </row>
   </sheetData>
@@ -527,7 +662,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -535,7 +670,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:9">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -545,47 +680,107 @@
       <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:4">
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
       <c r="A2" s="1" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="B2" t="n">
-        <v>0.4897850485067529</v>
+        <v>0.5554278761660133</v>
       </c>
       <c r="C2" t="n">
-        <v>0.4530989449405458</v>
+        <v>0.5503470475807263</v>
       </c>
       <c r="D2" t="n">
-        <v>0.4809401921118542</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
+        <v>0.6047967180350287</v>
+      </c>
+      <c r="E2" t="n">
+        <v>0.2936982279542833</v>
+      </c>
+      <c r="F2" t="n">
+        <v>0.06131674349908248</v>
+      </c>
+      <c r="G2" t="n">
+        <v>0.0002579369344195344</v>
+      </c>
+      <c r="H2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2" t="n">
+        <v>0.01229528113913593</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
       <c r="A3" s="1" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="B3" t="n">
-        <v>0.2112716258860468</v>
+        <v>0.1029781286706216</v>
       </c>
       <c r="C3" t="n">
-        <v>0.03669936526255049</v>
+        <v>0.04475699175913309</v>
       </c>
       <c r="D3" t="n">
-        <v>0.002922337870296237</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
+        <v>0.04596986541837332</v>
+      </c>
+      <c r="E3" t="n">
+        <v>0.00490418672236854</v>
+      </c>
+      <c r="F3" t="n">
+        <v>0.2421089282605493</v>
+      </c>
+      <c r="G3" t="n">
+        <v>0.005034612964128383</v>
+      </c>
+      <c r="H3" t="n">
+        <v>0.02393376594316402</v>
+      </c>
+      <c r="I3" t="n">
+        <v>0.1996670928521458</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
       <c r="A4" s="1" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="B4" t="n">
-        <v>0.03362526082761819</v>
+        <v>0.04456059601357413</v>
       </c>
       <c r="C4" t="n">
-        <v>0.01134181484461559</v>
+        <v>0.01417725635381229</v>
       </c>
       <c r="D4" t="n">
-        <v>0</v>
+        <v>0.09742188428181062</v>
+      </c>
+      <c r="E4" t="n">
+        <v>0.01669144191972818</v>
+      </c>
+      <c r="F4" t="n">
+        <v>0.006567216877041222</v>
+      </c>
+      <c r="G4" t="n">
+        <v>0.001732220759328852</v>
+      </c>
+      <c r="H4" t="n">
+        <v>0.1716231469871833</v>
+      </c>
+      <c r="I4" t="n">
+        <v>0.2722694117579186</v>
       </c>
     </row>
   </sheetData>

</xml_diff>